<commit_message>
progress at work, not tested
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\civy\Documents\Projects\GB Scheduler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\civy\Documents\GitHub\GBScheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B96638-D61B-43D7-8C05-106616B86920}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B39A8F9-7D48-4C6E-A668-2623ED80A326}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C32DB2AC-9E8F-457C-85BF-6FDE95A2D2B3}"/>
   </bookViews>
@@ -1205,8 +1205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D327494-BCA3-4254-A20D-43FDCA6D2DDE}">
   <dimension ref="A1:L796"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed method for keeping track of long rebar requirements
Changed the rebar object to now hold a list of locations and corrosponding area requirements at those locations
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\civy\Documents\GitHub\GBScheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B39A8F9-7D48-4C6E-A668-2623ED80A326}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45564A00-C126-4051-A6E1-7759D3D664E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C32DB2AC-9E8F-457C-85BF-6FDE95A2D2B3}"/>
   </bookViews>
@@ -656,9 +656,6 @@
     <t>Note: Deflections are calculated using effective moment of inertia of cracked sections.</t>
   </si>
   <si>
-    <t xml:space="preserve"> 29 - DETAILED REBAR</t>
-  </si>
-  <si>
     <t>Analysis Top</t>
   </si>
   <si>
@@ -714,6 +711,9 @@
   </si>
   <si>
     <t>35.3 - Detailed Deflections - Service Combination 3</t>
+  </si>
+  <si>
+    <t>29 - DETAILED REBAR</t>
   </si>
 </sst>
 </file>
@@ -1205,8 +1205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D327494-BCA3-4254-A20D-43FDCA6D2DDE}">
   <dimension ref="A1:L796"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="A369" workbookViewId="0">
+      <selection activeCell="D371" sqref="D371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8794,7 +8794,7 @@
     </row>
     <row r="371" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A371" s="2" t="s">
-        <v>207</v>
+        <v>226</v>
       </c>
     </row>
     <row r="372" spans="1:8" x14ac:dyDescent="0.25">
@@ -8813,22 +8813,22 @@
         <v>160</v>
       </c>
       <c r="C374" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D374" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="D374" s="5" t="s">
+      <c r="E374" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E374" s="5" t="s">
+      <c r="F374" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="F374" s="5" t="s">
+      <c r="G374" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="G374" s="5" t="s">
+      <c r="H374" s="5" t="s">
         <v>212</v>
-      </c>
-      <c r="H374" s="5" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="375" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9419,22 +9419,22 @@
         <v>160</v>
       </c>
       <c r="C399" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D399" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="D399" s="5" t="s">
+      <c r="E399" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E399" s="5" t="s">
+      <c r="F399" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="F399" s="5" t="s">
+      <c r="G399" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="G399" s="5" t="s">
+      <c r="H399" s="5" t="s">
         <v>212</v>
-      </c>
-      <c r="H399" s="5" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="400" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10025,22 +10025,22 @@
         <v>160</v>
       </c>
       <c r="C424" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D424" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="D424" s="5" t="s">
+      <c r="E424" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E424" s="5" t="s">
+      <c r="F424" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="F424" s="5" t="s">
+      <c r="G424" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="G424" s="5" t="s">
+      <c r="H424" s="5" t="s">
         <v>212</v>
-      </c>
-      <c r="H424" s="5" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="425" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10631,22 +10631,22 @@
         <v>160</v>
       </c>
       <c r="C449" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D449" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="D449" s="5" t="s">
+      <c r="E449" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E449" s="5" t="s">
+      <c r="F449" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="F449" s="5" t="s">
+      <c r="G449" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="G449" s="5" t="s">
+      <c r="H449" s="5" t="s">
         <v>212</v>
-      </c>
-      <c r="H449" s="5" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="450" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11226,7 +11226,7 @@
     </row>
     <row r="473" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A473" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="474" spans="1:8" x14ac:dyDescent="0.25">
@@ -11234,7 +11234,7 @@
     </row>
     <row r="475" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A475" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="476" spans="1:8" x14ac:dyDescent="0.25">
@@ -11242,7 +11242,7 @@
     </row>
     <row r="477" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A477" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="478" spans="1:8" x14ac:dyDescent="0.25">
@@ -11263,22 +11263,22 @@
         <v>160</v>
       </c>
       <c r="C480" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D480" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="D480" s="5" t="s">
+      <c r="E480" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E480" s="5" t="s">
+      <c r="F480" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="F480" s="5" t="s">
+      <c r="G480" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="G480" s="5" t="s">
+      <c r="H480" s="5" t="s">
         <v>221</v>
-      </c>
-      <c r="H480" s="5" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="481" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11921,22 +11921,22 @@
         <v>160</v>
       </c>
       <c r="C507" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D507" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="D507" s="5" t="s">
+      <c r="E507" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E507" s="5" t="s">
+      <c r="F507" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="F507" s="5" t="s">
+      <c r="G507" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="G507" s="5" t="s">
+      <c r="H507" s="5" t="s">
         <v>221</v>
-      </c>
-      <c r="H507" s="5" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="508" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12579,22 +12579,22 @@
         <v>160</v>
       </c>
       <c r="C534" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D534" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="D534" s="5" t="s">
+      <c r="E534" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E534" s="5" t="s">
+      <c r="F534" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="F534" s="5" t="s">
+      <c r="G534" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="G534" s="5" t="s">
+      <c r="H534" s="5" t="s">
         <v>221</v>
-      </c>
-      <c r="H534" s="5" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="535" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13237,22 +13237,22 @@
         <v>160</v>
       </c>
       <c r="C561" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D561" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="D561" s="5" t="s">
+      <c r="E561" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E561" s="5" t="s">
+      <c r="F561" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="F561" s="5" t="s">
+      <c r="G561" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="G561" s="5" t="s">
+      <c r="H561" s="5" t="s">
         <v>221</v>
-      </c>
-      <c r="H561" s="5" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="562" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13884,7 +13884,7 @@
     </row>
     <row r="587" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A587" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="588" spans="1:8" x14ac:dyDescent="0.25">
@@ -13892,7 +13892,7 @@
     </row>
     <row r="589" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A589" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="590" spans="1:8" x14ac:dyDescent="0.25">
@@ -13900,7 +13900,7 @@
     </row>
     <row r="591" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A591" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="592" spans="1:8" x14ac:dyDescent="0.25">
@@ -16608,7 +16608,7 @@
     </row>
     <row r="693" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A693" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="694" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>